<commit_message>
Removed old TEF files and added Ybus formation script
</commit_message>
<xml_diff>
--- a/Chandan_Work/MaPai/Ybus_matrix.xlsx
+++ b/Chandan_Work/MaPai/Ybus_matrix.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="57" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="608" uniqueCount="10">
   <si>
     <t>Row</t>
   </si>
@@ -98,9 +98,9 @@
     <col min="2" max="2" width="4.88671875" customWidth="true"/>
     <col min="3" max="3" width="4.88671875" customWidth="true"/>
     <col min="4" max="4" width="4.88671875" customWidth="true"/>
-    <col min="5" max="5" width="6.5546875" customWidth="true"/>
-    <col min="6" max="6" width="7.21875" customWidth="true"/>
-    <col min="7" max="7" width="7.21875" customWidth="true"/>
+    <col min="5" max="5" width="6.21875" customWidth="true"/>
+    <col min="6" max="6" width="6.21875" customWidth="true"/>
+    <col min="7" max="7" width="6.21875" customWidth="true"/>
     <col min="8" max="8" width="6.21875" customWidth="true"/>
     <col min="9" max="9" width="6.21875" customWidth="true"/>
     <col min="10" max="10" width="6.21875" customWidth="true"/>
@@ -248,13 +248,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="0">
-        <v>3.3073999999999999</v>
+        <v>3.3069999999999999</v>
       </c>
       <c r="F5" s="0">
-        <v>-1.3652</v>
+        <v>-1.365</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.9421999999999999</v>
+        <v>-1.9419999999999999</v>
       </c>
       <c r="H5" s="0">
         <v>0</v>
@@ -283,7 +283,7 @@
         <v>-1.365</v>
       </c>
       <c r="F6" s="0">
-        <v>3.8140000000000001</v>
+        <v>2.5529999999999999</v>
       </c>
       <c r="G6" s="0">
         <v>0</v>
@@ -388,7 +388,7 @@
         <v>-1.617</v>
       </c>
       <c r="I9" s="0">
-        <v>3.7410000000000001</v>
+        <v>2.7719999999999998</v>
       </c>
       <c r="J9" s="0">
         <v>-1.155</v>

</xml_diff>